<commit_message>
excel docs to excel folder
</commit_message>
<xml_diff>
--- a/excel/MLP_Results_in_Fuzzy_Generated_Dataset.xlsx
+++ b/excel/MLP_Results_in_Fuzzy_Generated_Dataset.xlsx
@@ -546,7 +546,7 @@
         <v>0.1736778509780632</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1141111122379027</v>
+        <v>0.09214447549927351</v>
       </c>
     </row>
     <row r="3">
@@ -590,7 +590,7 @@
         <v>0.7174718242740762</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7232420241177763</v>
+        <v>0.7133304808680634</v>
       </c>
     </row>
     <row r="4">
@@ -634,7 +634,7 @@
         <v>0.6405095945247496</v>
       </c>
       <c r="N4" t="n">
-        <v>0.3366158342762312</v>
+        <v>0.1867430863914004</v>
       </c>
     </row>
     <row r="5">
@@ -678,7 +678,7 @@
         <v>0.9414352360170024</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9586360456945368</v>
+        <v>0.9172663807733371</v>
       </c>
     </row>
     <row r="6">
@@ -722,7 +722,7 @@
         <v>0.1493776363242816</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.1104256237377928</v>
+        <v>0.0478416072194302</v>
       </c>
     </row>
     <row r="7">
@@ -766,7 +766,7 @@
         <v>0.7827505456633502</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8522600862107143</v>
+        <v>0.8080572038568468</v>
       </c>
     </row>
     <row r="8">
@@ -810,7 +810,7 @@
         <v>0.8531418237585843</v>
       </c>
       <c r="N8" t="n">
-        <v>0.6390657142412911</v>
+        <v>0.3475754853420566</v>
       </c>
     </row>
     <row r="9">
@@ -854,7 +854,7 @@
         <v>0.4303630102790368</v>
       </c>
       <c r="N9" t="n">
-        <v>0.448520698737132</v>
+        <v>0.3939991843685396</v>
       </c>
     </row>
     <row r="10">
@@ -898,7 +898,7 @@
         <v>0.8057257864076718</v>
       </c>
       <c r="N10" t="n">
-        <v>0.7764957859934003</v>
+        <v>0.7848627655621003</v>
       </c>
     </row>
     <row r="11">
@@ -942,7 +942,7 @@
         <v>-0.7307390552518273</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.6035025154487415</v>
+        <v>-0.6163653103806043</v>
       </c>
     </row>
     <row r="12">
@@ -986,7 +986,7 @@
         <v>0.8671631104276906</v>
       </c>
       <c r="N12" t="n">
-        <v>0.8673286699769863</v>
+        <v>0.8816816963470047</v>
       </c>
     </row>
     <row r="13">
@@ -1030,7 +1030,7 @@
         <v>0.8186365771850609</v>
       </c>
       <c r="N13" t="n">
-        <v>0.877172911909074</v>
+        <v>0.8506671522381259</v>
       </c>
     </row>
     <row r="14">
@@ -1074,7 +1074,7 @@
         <v>-0.2400419258905555</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.2845458496605166</v>
+        <v>-0.1686009795871576</v>
       </c>
     </row>
     <row r="15">
@@ -1118,7 +1118,7 @@
         <v>0.7927553701244862</v>
       </c>
       <c r="N15" t="n">
-        <v>0.7557159885838537</v>
+        <v>0.7760846055288393</v>
       </c>
     </row>
     <row r="16">
@@ -1162,7 +1162,7 @@
         <v>0.7603158913708737</v>
       </c>
       <c r="N16" t="n">
-        <v>0.7597402551198976</v>
+        <v>0.7632268076978712</v>
       </c>
     </row>
     <row r="17">
@@ -1206,7 +1206,7 @@
         <v>0.1287152483520124</v>
       </c>
       <c r="N17" t="n">
-        <v>0.3424721882066623</v>
+        <v>0.2169084040717104</v>
       </c>
     </row>
     <row r="18">
@@ -1250,7 +1250,7 @@
         <v>0.8083634986112384</v>
       </c>
       <c r="N18" t="n">
-        <v>0.853707495887234</v>
+        <v>0.8601130081057617</v>
       </c>
     </row>
     <row r="19">
@@ -1294,7 +1294,7 @@
         <v>0.461542053591235</v>
       </c>
       <c r="N19" t="n">
-        <v>0.6922207291221442</v>
+        <v>0.4557286941148584</v>
       </c>
     </row>
     <row r="20">
@@ -1338,7 +1338,7 @@
         <v>0.095190176378021</v>
       </c>
       <c r="N20" t="n">
-        <v>0.2247199182381246</v>
+        <v>0.1488502687133321</v>
       </c>
     </row>
     <row r="21">
@@ -1382,7 +1382,7 @@
         <v>-0.6001676436668545</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.4357522993354316</v>
+        <v>-0.3129015786196181</v>
       </c>
     </row>
     <row r="22">
@@ -1426,7 +1426,7 @@
         <v>0.8811256054547035</v>
       </c>
       <c r="N22" t="n">
-        <v>0.8869938039765589</v>
+        <v>0.8169368100434757</v>
       </c>
     </row>
     <row r="23">
@@ -1470,7 +1470,7 @@
         <v>-0.467525408816902</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.4168966796868146</v>
+        <v>-0.2231281780366557</v>
       </c>
     </row>
     <row r="24">
@@ -1514,7 +1514,7 @@
         <v>0.8295670664719411</v>
       </c>
       <c r="N24" t="n">
-        <v>0.8286833461274268</v>
+        <v>0.8289750516499481</v>
       </c>
     </row>
     <row r="25">
@@ -1558,7 +1558,7 @@
         <v>0.7449027457985314</v>
       </c>
       <c r="N25" t="n">
-        <v>0.7515110233672416</v>
+        <v>0.747772436732412</v>
       </c>
     </row>
     <row r="26">
@@ -1602,7 +1602,7 @@
         <v>0.5995583705743804</v>
       </c>
       <c r="N26" t="n">
-        <v>0.6894987915308841</v>
+        <v>0.6867408266915929</v>
       </c>
     </row>
     <row r="27">
@@ -1646,7 +1646,7 @@
         <v>0.1164519381885257</v>
       </c>
       <c r="N27" t="n">
-        <v>0.5196662020592836</v>
+        <v>0.235786324784693</v>
       </c>
     </row>
     <row r="28">
@@ -1690,7 +1690,7 @@
         <v>0.7671963949095978</v>
       </c>
       <c r="N28" t="n">
-        <v>0.7847973394484868</v>
+        <v>0.7869214906093415</v>
       </c>
     </row>
     <row r="29">
@@ -1734,7 +1734,7 @@
         <v>0.8435791683405595</v>
       </c>
       <c r="N29" t="n">
-        <v>0.8569434037098406</v>
+        <v>0.8776932402966361</v>
       </c>
     </row>
     <row r="30">
@@ -1778,7 +1778,7 @@
         <v>0.5491128260281543</v>
       </c>
       <c r="N30" t="n">
-        <v>0.5269097696671602</v>
+        <v>0.507133080671357</v>
       </c>
     </row>
     <row r="31">
@@ -1822,7 +1822,7 @@
         <v>0.1111147758783954</v>
       </c>
       <c r="N31" t="n">
-        <v>0.09177452087401837</v>
+        <v>0.06380882421885359</v>
       </c>
     </row>
     <row r="32">
@@ -1866,7 +1866,7 @@
         <v>0.8040315733364831</v>
       </c>
       <c r="N32" t="n">
-        <v>0.7944442299881552</v>
+        <v>0.8190268227845268</v>
       </c>
     </row>
     <row r="33">
@@ -1910,7 +1910,7 @@
         <v>0.7917728430223494</v>
       </c>
       <c r="N33" t="n">
-        <v>0.5867719197372155</v>
+        <v>0.5080114913767306</v>
       </c>
     </row>
     <row r="34">
@@ -1954,7 +1954,7 @@
         <v>-0.7385820097184317</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.6558424617941905</v>
+        <v>-0.6667680232741825</v>
       </c>
     </row>
     <row r="35">
@@ -1998,7 +1998,7 @@
         <v>0.8096104008885238</v>
       </c>
       <c r="N35" t="n">
-        <v>0.7954887448247739</v>
+        <v>0.8374558797216545</v>
       </c>
     </row>
     <row r="36">
@@ -2042,7 +2042,7 @@
         <v>0.8191195452880168</v>
       </c>
       <c r="N36" t="n">
-        <v>0.8180196389167905</v>
+        <v>0.7803084552025337</v>
       </c>
     </row>
     <row r="37">
@@ -2086,7 +2086,7 @@
         <v>0.8232726908389609</v>
       </c>
       <c r="N37" t="n">
-        <v>0.8097799950098702</v>
+        <v>0.8016491840960762</v>
       </c>
     </row>
     <row r="38">
@@ -2130,7 +2130,7 @@
         <v>-0.5954543075170342</v>
       </c>
       <c r="N38" t="n">
-        <v>-0.4802834714419927</v>
+        <v>-0.4090361324407878</v>
       </c>
     </row>
     <row r="39">
@@ -2174,7 +2174,7 @@
         <v>0.8597495003171647</v>
       </c>
       <c r="N39" t="n">
-        <v>0.8613285799301483</v>
+        <v>0.8748220758983363</v>
       </c>
     </row>
     <row r="40">
@@ -2218,7 +2218,7 @@
         <v>0.7942587076652455</v>
       </c>
       <c r="N40" t="n">
-        <v>0.757931239384363</v>
+        <v>0.7764017764420292</v>
       </c>
     </row>
     <row r="41">
@@ -2262,7 +2262,7 @@
         <v>-0.6048123557839027</v>
       </c>
       <c r="N41" t="n">
-        <v>-0.4984533320768902</v>
+        <v>-0.2076573747778765</v>
       </c>
     </row>
     <row r="42">
@@ -2306,7 +2306,7 @@
         <v>0.5975609030808818</v>
       </c>
       <c r="N42" t="n">
-        <v>0.2390967457202782</v>
+        <v>0.06192729972504962</v>
       </c>
     </row>
     <row r="43">
@@ -2350,7 +2350,7 @@
         <v>-0.1424500709309019</v>
       </c>
       <c r="N43" t="n">
-        <v>-0.1022259924367946</v>
+        <v>-0.04446053094495339</v>
       </c>
     </row>
     <row r="44">
@@ -2394,7 +2394,7 @@
         <v>-0.0556038660041097</v>
       </c>
       <c r="N44" t="n">
-        <v>0.2970409932739079</v>
+        <v>0.1704080563655692</v>
       </c>
     </row>
     <row r="45">
@@ -2438,7 +2438,7 @@
         <v>0.8832512774573102</v>
       </c>
       <c r="N45" t="n">
-        <v>0.6924017670554633</v>
+        <v>0.7100685107088768</v>
       </c>
     </row>
     <row r="46">
@@ -2482,7 +2482,7 @@
         <v>-0.5869480239984458</v>
       </c>
       <c r="N46" t="n">
-        <v>-0.4061635270064128</v>
+        <v>-0.2478105504539347</v>
       </c>
     </row>
     <row r="47">
@@ -2526,7 +2526,7 @@
         <v>0.5236381151792733</v>
       </c>
       <c r="N47" t="n">
-        <v>0.5659744131016269</v>
+        <v>0.6158885227616361</v>
       </c>
     </row>
     <row r="48">
@@ -2570,7 +2570,7 @@
         <v>-0.6246275041942413</v>
       </c>
       <c r="N48" t="n">
-        <v>-0.456255032080375</v>
+        <v>-0.3849073892666869</v>
       </c>
     </row>
     <row r="49">
@@ -2614,7 +2614,7 @@
         <v>0.0448482038000717</v>
       </c>
       <c r="N49" t="n">
-        <v>-0.1293010418570461</v>
+        <v>-0.1530326420919571</v>
       </c>
     </row>
     <row r="50">
@@ -2658,7 +2658,7 @@
         <v>0.1877876531134831</v>
       </c>
       <c r="N50" t="n">
-        <v>0.3167598374007654</v>
+        <v>0.3166326347721828</v>
       </c>
     </row>
     <row r="51">
@@ -2702,7 +2702,7 @@
         <v>0.8939342311067586</v>
       </c>
       <c r="N51" t="n">
-        <v>0.8986265114325892</v>
+        <v>0.9011175797993558</v>
       </c>
     </row>
     <row r="52">
@@ -2746,7 +2746,7 @@
         <v>-0.0096982680498709</v>
       </c>
       <c r="N52" t="n">
-        <v>0.2961660135750804</v>
+        <v>0.002409525876759688</v>
       </c>
     </row>
     <row r="53">
@@ -2790,7 +2790,7 @@
         <v>0.6624474105300963</v>
       </c>
       <c r="N53" t="n">
-        <v>0.7968435551033409</v>
+        <v>0.7769120568875678</v>
       </c>
     </row>
     <row r="54">
@@ -2834,7 +2834,7 @@
         <v>0.8885870199743783</v>
       </c>
       <c r="N54" t="n">
-        <v>0.8638753342076118</v>
+        <v>0.8695669433959041</v>
       </c>
     </row>
     <row r="55">
@@ -2878,7 +2878,7 @@
         <v>0.7550372582033518</v>
       </c>
       <c r="N55" t="n">
-        <v>0.2844423276483448</v>
+        <v>0.1352703879237292</v>
       </c>
     </row>
     <row r="56">
@@ -2922,7 +2922,7 @@
         <v>0.8836066876006297</v>
       </c>
       <c r="N56" t="n">
-        <v>0.8612698458076949</v>
+        <v>0.861303831762765</v>
       </c>
     </row>
     <row r="57">
@@ -2966,7 +2966,7 @@
         <v>0.9235651581296336</v>
       </c>
       <c r="N57" t="n">
-        <v>0.9147213965752446</v>
+        <v>0.9228256454700889</v>
       </c>
     </row>
     <row r="58">
@@ -3010,7 +3010,7 @@
         <v>0.2394915391695954</v>
       </c>
       <c r="N58" t="n">
-        <v>0.6183907097677552</v>
+        <v>0.5095723295435708</v>
       </c>
     </row>
     <row r="59">
@@ -3054,7 +3054,7 @@
         <v>0.3105649393880524</v>
       </c>
       <c r="N59" t="n">
-        <v>0.5808441373600561</v>
+        <v>0.4281454587065712</v>
       </c>
     </row>
     <row r="60">
@@ -3098,7 +3098,7 @@
         <v>-0.68402055768224</v>
       </c>
       <c r="N60" t="n">
-        <v>-0.611678554629581</v>
+        <v>-0.5780521027488824</v>
       </c>
     </row>
     <row r="61">
@@ -3142,7 +3142,7 @@
         <v>0.800797341861952</v>
       </c>
       <c r="N61" t="n">
-        <v>0.8308871258406073</v>
+        <v>0.7997190759305847</v>
       </c>
     </row>
     <row r="62">
@@ -3186,7 +3186,7 @@
         <v>-0.6453408149083908</v>
       </c>
       <c r="N62" t="n">
-        <v>-0.5653873342516095</v>
+        <v>-0.4637541461311648</v>
       </c>
     </row>
     <row r="63">
@@ -3230,7 +3230,7 @@
         <v>0.6372287494176876</v>
       </c>
       <c r="N63" t="n">
-        <v>0.7238985252290917</v>
+        <v>0.7563035841819538</v>
       </c>
     </row>
     <row r="64">
@@ -3274,7 +3274,7 @@
         <v>-0.7593449220841938</v>
       </c>
       <c r="N64" t="n">
-        <v>-0.6710192838129416</v>
+        <v>-0.6148866657391917</v>
       </c>
     </row>
     <row r="65">
@@ -3318,7 +3318,7 @@
         <v>0.2605083161279985</v>
       </c>
       <c r="N65" t="n">
-        <v>0.3957834233051438</v>
+        <v>0.2217743265893583</v>
       </c>
     </row>
     <row r="66">
@@ -3362,7 +3362,7 @@
         <v>0.4279472208204202</v>
       </c>
       <c r="N66" t="n">
-        <v>0.3431200235021991</v>
+        <v>0.2216972482576333</v>
       </c>
     </row>
     <row r="67">
@@ -3406,7 +3406,7 @@
         <v>0.8715277186287771</v>
       </c>
       <c r="N67" t="n">
-        <v>0.8635697864996444</v>
+        <v>0.88178164252786</v>
       </c>
     </row>
     <row r="68">
@@ -3450,7 +3450,7 @@
         <v>0.6320605069828524</v>
       </c>
       <c r="N68" t="n">
-        <v>0.7317145183778421</v>
+        <v>0.7119112139209167</v>
       </c>
     </row>
     <row r="69">
@@ -3494,7 +3494,7 @@
         <v>0.6359019119500453</v>
       </c>
       <c r="N69" t="n">
-        <v>0.576866381509872</v>
+        <v>0.6790462184718907</v>
       </c>
     </row>
     <row r="70">
@@ -3538,7 +3538,7 @@
         <v>0.8534439978730277</v>
       </c>
       <c r="N70" t="n">
-        <v>0.8359132767817925</v>
+        <v>0.8551006921816882</v>
       </c>
     </row>
     <row r="71">
@@ -3582,7 +3582,7 @@
         <v>0.9046668603812892</v>
       </c>
       <c r="N71" t="n">
-        <v>0.9327145797896027</v>
+        <v>0.926257154563065</v>
       </c>
     </row>
     <row r="72">
@@ -3626,7 +3626,7 @@
         <v>0.865869451049894</v>
       </c>
       <c r="N72" t="n">
-        <v>0.8727306551940807</v>
+        <v>0.8587324549049338</v>
       </c>
     </row>
     <row r="73">
@@ -3670,7 +3670,7 @@
         <v>-0.6036404071008991</v>
       </c>
       <c r="N73" t="n">
-        <v>-0.4106193677034897</v>
+        <v>-0.2918470482912343</v>
       </c>
     </row>
     <row r="74">
@@ -3714,7 +3714,7 @@
         <v>0.9260487068467554</v>
       </c>
       <c r="N74" t="n">
-        <v>1</v>
+        <v>0.9645794725677156</v>
       </c>
     </row>
     <row r="75">
@@ -3758,7 +3758,7 @@
         <v>0.799904644510518</v>
       </c>
       <c r="N75" t="n">
-        <v>0.828169834097472</v>
+        <v>0.8358918883818753</v>
       </c>
     </row>
     <row r="76">
@@ -3802,7 +3802,7 @@
         <v>0.8647171967262132</v>
       </c>
       <c r="N76" t="n">
-        <v>0.8690636231352659</v>
+        <v>0.8771783544094083</v>
       </c>
     </row>
     <row r="77">
@@ -3846,7 +3846,7 @@
         <v>0.6699995299450422</v>
       </c>
       <c r="N77" t="n">
-        <v>0.6684505649059376</v>
+        <v>0.7228782376701955</v>
       </c>
     </row>
     <row r="78">
@@ -3890,7 +3890,7 @@
         <v>-0.5690057469361014</v>
       </c>
       <c r="N78" t="n">
-        <v>-0.3757808264819515</v>
+        <v>-0.3430929978920452</v>
       </c>
     </row>
     <row r="79">
@@ -3934,7 +3934,7 @@
         <v>-0.7474748592658077</v>
       </c>
       <c r="N79" t="n">
-        <v>-0.7904872725266726</v>
+        <v>-0.938700834969444</v>
       </c>
     </row>
     <row r="80">
@@ -3978,7 +3978,7 @@
         <v>0.112298438929794</v>
       </c>
       <c r="N80" t="n">
-        <v>0.4432853285702463</v>
+        <v>0.3398664815604842</v>
       </c>
     </row>
     <row r="81">
@@ -4022,7 +4022,7 @@
         <v>-0.0212677870395506</v>
       </c>
       <c r="N81" t="n">
-        <v>0.3341154292672655</v>
+        <v>0.3926237249924676</v>
       </c>
     </row>
     <row r="82">
@@ -4066,7 +4066,7 @@
         <v>0.8378187977180528</v>
       </c>
       <c r="N82" t="n">
-        <v>0.8547279951991436</v>
+        <v>0.870087074430324</v>
       </c>
     </row>
     <row r="83">
@@ -4110,7 +4110,7 @@
         <v>0.5447930286830892</v>
       </c>
       <c r="N83" t="n">
-        <v>0.340033856223222</v>
+        <v>0.4664065927364912</v>
       </c>
     </row>
     <row r="84">
@@ -4154,7 +4154,7 @@
         <v>0.62625791128283</v>
       </c>
       <c r="N84" t="n">
-        <v>0.6477933512781415</v>
+        <v>0.7471018981104662</v>
       </c>
     </row>
     <row r="85">
@@ -4198,7 +4198,7 @@
         <v>0.803240979021019</v>
       </c>
       <c r="N85" t="n">
-        <v>0.7904542638620542</v>
+        <v>0.7889109533798219</v>
       </c>
     </row>
     <row r="86">
@@ -4242,7 +4242,7 @@
         <v>0.0200382060092032</v>
       </c>
       <c r="N86" t="n">
-        <v>-0.1344010021222359</v>
+        <v>-0.0937282160141627</v>
       </c>
     </row>
     <row r="87">
@@ -4286,7 +4286,7 @@
         <v>0.6262657969362001</v>
       </c>
       <c r="N87" t="n">
-        <v>0.7043775224904207</v>
+        <v>0.77043608570431</v>
       </c>
     </row>
     <row r="88">
@@ -4330,7 +4330,7 @@
         <v>-0.8181189796368755</v>
       </c>
       <c r="N88" t="n">
-        <v>-0.6908115788139212</v>
+        <v>-0.812598572223373</v>
       </c>
     </row>
     <row r="89">
@@ -4374,7 +4374,7 @@
         <v>0.8775325737230137</v>
       </c>
       <c r="N89" t="n">
-        <v>0.8824142037051657</v>
+        <v>0.9131444383906124</v>
       </c>
     </row>
     <row r="90">
@@ -4418,7 +4418,7 @@
         <v>-0.8482494021801671</v>
       </c>
       <c r="N90" t="n">
-        <v>-0.9063132821897876</v>
+        <v>-0.8345580360552761</v>
       </c>
     </row>
     <row r="91">
@@ -4462,7 +4462,7 @@
         <v>-0.2666127070995717</v>
       </c>
       <c r="N91" t="n">
-        <v>-0.04530067153094779</v>
+        <v>-0.2317136034846353</v>
       </c>
     </row>
     <row r="92">
@@ -4506,7 +4506,7 @@
         <v>0.9015348236369471</v>
       </c>
       <c r="N92" t="n">
-        <v>0.9173557876134467</v>
+        <v>0.9298100601735494</v>
       </c>
     </row>
     <row r="93">
@@ -4550,7 +4550,7 @@
         <v>-0.5933402556025952</v>
       </c>
       <c r="N93" t="n">
-        <v>-0.4492371263668544</v>
+        <v>-0.4046327591959981</v>
       </c>
     </row>
     <row r="94">
@@ -4594,7 +4594,7 @@
         <v>0.1246358420613772</v>
       </c>
       <c r="N94" t="n">
-        <v>0.09203007015166915</v>
+        <v>0.2960875286992765</v>
       </c>
     </row>
     <row r="95">
@@ -4638,7 +4638,7 @@
         <v>0.8002990524371381</v>
       </c>
       <c r="N95" t="n">
-        <v>0.7295079201610066</v>
+        <v>0.7696128505847886</v>
       </c>
     </row>
     <row r="96">
@@ -4682,7 +4682,7 @@
         <v>0.6614785212469462</v>
       </c>
       <c r="N96" t="n">
-        <v>0.2074798093893045</v>
+        <v>0.3167849213556293</v>
       </c>
     </row>
     <row r="97">
@@ -4726,7 +4726,7 @@
         <v>0.8057840545919791</v>
       </c>
       <c r="N97" t="n">
-        <v>0.9089453152882784</v>
+        <v>0.8735967672608178</v>
       </c>
     </row>
     <row r="98">
@@ -4770,7 +4770,7 @@
         <v>0.267176333665084</v>
       </c>
       <c r="N98" t="n">
-        <v>0.2546694233017182</v>
+        <v>0.1433497131953225</v>
       </c>
     </row>
     <row r="99">
@@ -4814,7 +4814,7 @@
         <v>0.8554840164125541</v>
       </c>
       <c r="N99" t="n">
-        <v>0.9265775983426318</v>
+        <v>0.8926439908848435</v>
       </c>
     </row>
     <row r="100">
@@ -4858,7 +4858,7 @@
         <v>0.6124539261991486</v>
       </c>
       <c r="N100" t="n">
-        <v>0.6838278009839925</v>
+        <v>0.6967777053879624</v>
       </c>
     </row>
     <row r="101">
@@ -4902,7 +4902,7 @@
         <v>0.8121707585851295</v>
       </c>
       <c r="N101" t="n">
-        <v>0.774955859991554</v>
+        <v>0.8127240723587944</v>
       </c>
     </row>
     <row r="102">
@@ -4946,7 +4946,7 @@
         <v>-0.3918957178982818</v>
       </c>
       <c r="N102" t="n">
-        <v>-0.4294524365815958</v>
+        <v>-0.2982397340289907</v>
       </c>
     </row>
     <row r="103">
@@ -4990,7 +4990,7 @@
         <v>0.8271654986854226</v>
       </c>
       <c r="N103" t="n">
-        <v>0.8266062770985482</v>
+        <v>0.8117909170664751</v>
       </c>
     </row>
     <row r="104">
@@ -5034,7 +5034,7 @@
         <v>0.6500038448222469</v>
       </c>
       <c r="N104" t="n">
-        <v>0.5225075750399166</v>
+        <v>0.6261406518390427</v>
       </c>
     </row>
     <row r="105">
@@ -5078,7 +5078,7 @@
         <v>-0.5429308696993087</v>
       </c>
       <c r="N105" t="n">
-        <v>-0.461483748907154</v>
+        <v>-0.4540288132770774</v>
       </c>
     </row>
     <row r="106">
@@ -5122,7 +5122,7 @@
         <v>0.8983763849722117</v>
       </c>
       <c r="N106" t="n">
-        <v>0.9057210430438802</v>
+        <v>0.9006267833617979</v>
       </c>
     </row>
     <row r="107">
@@ -5166,7 +5166,7 @@
         <v>-0.2914657238152308</v>
       </c>
       <c r="N107" t="n">
-        <v>0.4124497384925594</v>
+        <v>0.3352818157194204</v>
       </c>
     </row>
     <row r="108">
@@ -5210,7 +5210,7 @@
         <v>-0.7143509004531791</v>
       </c>
       <c r="N108" t="n">
-        <v>-0.6736146998076492</v>
+        <v>-0.5699036678517605</v>
       </c>
     </row>
     <row r="109">
@@ -5254,7 +5254,7 @@
         <v>-0.6752749758056793</v>
       </c>
       <c r="N109" t="n">
-        <v>-0.6646171508508115</v>
+        <v>-0.6681943976759345</v>
       </c>
     </row>
     <row r="110">
@@ -5298,7 +5298,7 @@
         <v>0.6308097681265178</v>
       </c>
       <c r="N110" t="n">
-        <v>0.7747869496774326</v>
+        <v>0.7933265196010896</v>
       </c>
     </row>
     <row r="111">
@@ -5342,7 +5342,7 @@
         <v>0.5956826320656641</v>
       </c>
       <c r="N111" t="n">
-        <v>0.6221488299800644</v>
+        <v>0.6699751595494845</v>
       </c>
     </row>
     <row r="112">
@@ -5386,7 +5386,7 @@
         <v>-0.1593835940177428</v>
       </c>
       <c r="N112" t="n">
-        <v>-0.2283982863836332</v>
+        <v>-0.08513768981922043</v>
       </c>
     </row>
     <row r="113">
@@ -5430,7 +5430,7 @@
         <v>0.06283146081773761</v>
       </c>
       <c r="N113" t="n">
-        <v>0.3107736269906686</v>
+        <v>0.07501081531339876</v>
       </c>
     </row>
     <row r="114">
@@ -5474,7 +5474,7 @@
         <v>0.7296741426278416</v>
       </c>
       <c r="N114" t="n">
-        <v>0.7276899940597721</v>
+        <v>0.7716283312022965</v>
       </c>
     </row>
     <row r="115">
@@ -5518,7 +5518,7 @@
         <v>0.7494417903158634</v>
       </c>
       <c r="N115" t="n">
-        <v>0.734224769661037</v>
+        <v>0.7498317749054475</v>
       </c>
     </row>
     <row r="116">
@@ -5562,7 +5562,7 @@
         <v>0.8522040479554038</v>
       </c>
       <c r="N116" t="n">
-        <v>0.8269110269703587</v>
+        <v>0.8337698337976305</v>
       </c>
     </row>
     <row r="117">
@@ -5606,7 +5606,7 @@
         <v>-0.2283713874362877</v>
       </c>
       <c r="N117" t="n">
-        <v>-0.36168734916905</v>
+        <v>-0.128517231887368</v>
       </c>
     </row>
     <row r="118">
@@ -5650,7 +5650,7 @@
         <v>-0.682663361959934</v>
       </c>
       <c r="N118" t="n">
-        <v>-0.6495875172615371</v>
+        <v>-0.7058905128388145</v>
       </c>
     </row>
     <row r="119">
@@ -5694,7 +5694,7 @@
         <v>-0.1055638342778725</v>
       </c>
       <c r="N119" t="n">
-        <v>0.1827919303845288</v>
+        <v>0.1706136109970354</v>
       </c>
     </row>
     <row r="120">
@@ -5738,7 +5738,7 @@
         <v>-0.637679803562103</v>
       </c>
       <c r="N120" t="n">
-        <v>-0.6089081040087007</v>
+        <v>-0.5848597244466255</v>
       </c>
     </row>
     <row r="121">
@@ -5782,7 +5782,7 @@
         <v>0.0038273643098687</v>
       </c>
       <c r="N121" t="n">
-        <v>-0.05060395755990828</v>
+        <v>-0.008890283403318433</v>
       </c>
     </row>
     <row r="122">
@@ -5826,7 +5826,7 @@
         <v>-0.1598177006632067</v>
       </c>
       <c r="N122" t="n">
-        <v>-0.1582168267614983</v>
+        <v>0.02277528681378183</v>
       </c>
     </row>
     <row r="123">
@@ -5870,7 +5870,7 @@
         <v>0.8202919840367802</v>
       </c>
       <c r="N123" t="n">
-        <v>0.6735460924031929</v>
+        <v>0.6905701517727287</v>
       </c>
     </row>
     <row r="124">
@@ -5914,7 +5914,7 @@
         <v>0.8614986185535128</v>
       </c>
       <c r="N124" t="n">
-        <v>0.7212962934942294</v>
+        <v>0.6970060926424051</v>
       </c>
     </row>
     <row r="125">
@@ -5958,7 +5958,7 @@
         <v>0.8118157908034039</v>
       </c>
       <c r="N125" t="n">
-        <v>0.8081771109081853</v>
+        <v>0.8112590198078429</v>
       </c>
     </row>
     <row r="126">
@@ -6002,7 +6002,7 @@
         <v>-0.7554747738772086</v>
       </c>
       <c r="N126" t="n">
-        <v>-0.7710008558700249</v>
+        <v>-0.6381164340603315</v>
       </c>
     </row>
     <row r="127">
@@ -6046,7 +6046,7 @@
         <v>0.4216521286600801</v>
       </c>
       <c r="N127" t="n">
-        <v>0.3074886496805421</v>
+        <v>0.1046759345448778</v>
       </c>
     </row>
     <row r="128">
@@ -6090,7 +6090,7 @@
         <v>0.8955158202034835</v>
       </c>
       <c r="N128" t="n">
-        <v>0.9385274324905362</v>
+        <v>0.9009678995309978</v>
       </c>
     </row>
     <row r="129">
@@ -6134,7 +6134,7 @@
         <v>0.6497682481809143</v>
       </c>
       <c r="N129" t="n">
-        <v>0.7326690500377109</v>
+        <v>0.7673298772109394</v>
       </c>
     </row>
     <row r="130">
@@ -6178,7 +6178,7 @@
         <v>-0.8014656456508203</v>
       </c>
       <c r="N130" t="n">
-        <v>-0.7405743909573443</v>
+        <v>-0.8439360305935056</v>
       </c>
     </row>
     <row r="131">
@@ -6222,7 +6222,7 @@
         <v>0.8377669030448921</v>
       </c>
       <c r="N131" t="n">
-        <v>0.846537333917159</v>
+        <v>0.7971328044050259</v>
       </c>
     </row>
     <row r="132">
@@ -6266,7 +6266,7 @@
         <v>0.8162651758887149</v>
       </c>
       <c r="N132" t="n">
-        <v>0.812263266213197</v>
+        <v>0.8184809472548935</v>
       </c>
     </row>
     <row r="133">
@@ -6310,7 +6310,7 @@
         <v>0.5916804631195333</v>
       </c>
       <c r="N133" t="n">
-        <v>0.717507111082558</v>
+        <v>0.6986844953536713</v>
       </c>
     </row>
     <row r="134">
@@ -6354,7 +6354,7 @@
         <v>-0.689359086185134</v>
       </c>
       <c r="N134" t="n">
-        <v>-0.5957740341370464</v>
+        <v>-0.5317460330917044</v>
       </c>
     </row>
     <row r="135">
@@ -6398,7 +6398,7 @@
         <v>0.7769186629963599</v>
       </c>
       <c r="N135" t="n">
-        <v>0.7840047889928565</v>
+        <v>0.7424439793206207</v>
       </c>
     </row>
     <row r="136">
@@ -6442,7 +6442,7 @@
         <v>0.7870076105513747</v>
       </c>
       <c r="N136" t="n">
-        <v>0.7835684817705527</v>
+        <v>0.7863036707075808</v>
       </c>
     </row>
     <row r="137">
@@ -6486,7 +6486,7 @@
         <v>0.8118935346970153</v>
       </c>
       <c r="N137" t="n">
-        <v>0.8138488652933156</v>
+        <v>0.8239353709856976</v>
       </c>
     </row>
     <row r="138">
@@ -6530,7 +6530,7 @@
         <v>0.5254581748972803</v>
       </c>
       <c r="N138" t="n">
-        <v>0.5624824933954968</v>
+        <v>0.4605640169438341</v>
       </c>
     </row>
     <row r="139">
@@ -6574,7 +6574,7 @@
         <v>0.4489245887780391</v>
       </c>
       <c r="N139" t="n">
-        <v>0.08226880983404149</v>
+        <v>0.1937258812056301</v>
       </c>
     </row>
     <row r="140">
@@ -6618,7 +6618,7 @@
         <v>-0.570543411551818</v>
       </c>
       <c r="N140" t="n">
-        <v>-0.6264034436546694</v>
+        <v>-0.6229755255683326</v>
       </c>
     </row>
     <row r="141">
@@ -6662,7 +6662,7 @@
         <v>0.315656816216648</v>
       </c>
       <c r="N141" t="n">
-        <v>0.2478833830949031</v>
+        <v>0.4179100293712324</v>
       </c>
     </row>
     <row r="142">
@@ -6706,7 +6706,7 @@
         <v>-0.0304003330922369</v>
       </c>
       <c r="N142" t="n">
-        <v>0.02364819886771392</v>
+        <v>-0.01089029325403501</v>
       </c>
     </row>
     <row r="143">
@@ -6750,7 +6750,7 @@
         <v>0.4958957437897807</v>
       </c>
       <c r="N143" t="n">
-        <v>0.5087775124361442</v>
+        <v>0.3788510054749001</v>
       </c>
     </row>
     <row r="144">
@@ -6794,7 +6794,7 @@
         <v>-0.8394143871452177</v>
       </c>
       <c r="N144" t="n">
-        <v>-0.9381363895811784</v>
+        <v>-0.8851974886077237</v>
       </c>
     </row>
     <row r="145">
@@ -6838,7 +6838,7 @@
         <v>0.0703635482236441</v>
       </c>
       <c r="N145" t="n">
-        <v>-0.02436403183250489</v>
+        <v>0.2489757378001255</v>
       </c>
     </row>
     <row r="146">
@@ -6882,7 +6882,7 @@
         <v>-0.6521147659984303</v>
       </c>
       <c r="N146" t="n">
-        <v>-0.660237054967038</v>
+        <v>-0.6124203367270736</v>
       </c>
     </row>
     <row r="147">
@@ -6926,7 +6926,7 @@
         <v>0.8205774845112925</v>
       </c>
       <c r="N147" t="n">
-        <v>0.6457010972050837</v>
+        <v>0.7150804698498168</v>
       </c>
     </row>
     <row r="148">
@@ -6970,7 +6970,7 @@
         <v>0.7576394755404968</v>
       </c>
       <c r="N148" t="n">
-        <v>0.7536550224998078</v>
+        <v>0.7838795990166676</v>
       </c>
     </row>
     <row r="149">
@@ -7014,7 +7014,7 @@
         <v>0.7597651876757665</v>
       </c>
       <c r="N149" t="n">
-        <v>0.6534740525585172</v>
+        <v>0.6717397510882359</v>
       </c>
     </row>
     <row r="150">
@@ -7058,7 +7058,7 @@
         <v>-0.0354947221813832</v>
       </c>
       <c r="N150" t="n">
-        <v>-0.1989835052477223</v>
+        <v>-0.005573582959990442</v>
       </c>
     </row>
     <row r="151">
@@ -7102,7 +7102,7 @@
         <v>-0.5732395489995721</v>
       </c>
       <c r="N151" t="n">
-        <v>-0.4087457075163288</v>
+        <v>-0.2874741313162561</v>
       </c>
     </row>
     <row r="152">
@@ -7146,7 +7146,7 @@
         <v>0.7679227898296676</v>
       </c>
       <c r="N152" t="n">
-        <v>0.4326558037433222</v>
+        <v>0.381584521799974</v>
       </c>
     </row>
     <row r="153">
@@ -7190,7 +7190,7 @@
         <v>0.8510205337389072</v>
       </c>
       <c r="N153" t="n">
-        <v>0.8537415622547904</v>
+        <v>0.8642813973017118</v>
       </c>
     </row>
     <row r="154">
@@ -7234,7 +7234,7 @@
         <v>0.7666570423871293</v>
       </c>
       <c r="N154" t="n">
-        <v>0.7769424825435829</v>
+        <v>0.8026396140308076</v>
       </c>
     </row>
     <row r="155">
@@ -7278,7 +7278,7 @@
         <v>0.6077262734292631</v>
       </c>
       <c r="N155" t="n">
-        <v>0.7334886595887802</v>
+        <v>0.677218029623583</v>
       </c>
     </row>
     <row r="156">
@@ -7322,7 +7322,7 @@
         <v>0.9082659632004028</v>
       </c>
       <c r="N156" t="n">
-        <v>0.9231009004402158</v>
+        <v>0.9251779574621261</v>
       </c>
     </row>
     <row r="157">
@@ -7366,7 +7366,7 @@
         <v>0.827273767179836</v>
       </c>
       <c r="N157" t="n">
-        <v>0.8752878277832502</v>
+        <v>0.7992721162004049</v>
       </c>
     </row>
     <row r="158">
@@ -7410,7 +7410,7 @@
         <v>-0.2060627908644731</v>
       </c>
       <c r="N158" t="n">
-        <v>-0.2534738866810386</v>
+        <v>-0.2062214684244251</v>
       </c>
     </row>
     <row r="159">
@@ -7454,7 +7454,7 @@
         <v>0.8297657977596389</v>
       </c>
       <c r="N159" t="n">
-        <v>0.8075832479664112</v>
+        <v>0.8412628492711354</v>
       </c>
     </row>
     <row r="160">
@@ -7498,7 +7498,7 @@
         <v>0.9054903936117732</v>
       </c>
       <c r="N160" t="n">
-        <v>0.7763520685633103</v>
+        <v>0.8206471862907539</v>
       </c>
     </row>
     <row r="161">
@@ -7542,7 +7542,7 @@
         <v>0.7317282676338609</v>
       </c>
       <c r="N161" t="n">
-        <v>0.6291438075841976</v>
+        <v>0.4671003210653695</v>
       </c>
     </row>
     <row r="162">
@@ -7586,7 +7586,7 @@
         <v>0.5404446450023527</v>
       </c>
       <c r="N162" t="n">
-        <v>0.6501258026796661</v>
+        <v>0.7364625244406021</v>
       </c>
     </row>
     <row r="163">
@@ -7630,7 +7630,7 @@
         <v>-0.7628726739277146</v>
       </c>
       <c r="N163" t="n">
-        <v>-0.6245358795604952</v>
+        <v>-0.8538933242189514</v>
       </c>
     </row>
     <row r="164">
@@ -7674,7 +7674,7 @@
         <v>-0.0969153042563379</v>
       </c>
       <c r="N164" t="n">
-        <v>0.4701696039188459</v>
+        <v>0.5154347947294271</v>
       </c>
     </row>
     <row r="165">
@@ -7718,7 +7718,7 @@
         <v>-0.6716844256314339</v>
       </c>
       <c r="N165" t="n">
-        <v>-0.5116149256559273</v>
+        <v>-0.7358985783712958</v>
       </c>
     </row>
     <row r="166">
@@ -7762,7 +7762,7 @@
         <v>-0.2347730679348304</v>
       </c>
       <c r="N166" t="n">
-        <v>-0.277401227076203</v>
+        <v>-0.1524783464791934</v>
       </c>
     </row>
     <row r="167">
@@ -7806,7 +7806,7 @@
         <v>-0.0970624888884704</v>
       </c>
       <c r="N167" t="n">
-        <v>-0.0698690659365946</v>
+        <v>-0.02841611980266079</v>
       </c>
     </row>
     <row r="168">
@@ -7850,7 +7850,7 @@
         <v>0.7411391043759472</v>
       </c>
       <c r="N168" t="n">
-        <v>0.6681543142976042</v>
+        <v>0.6811559165887601</v>
       </c>
     </row>
     <row r="169">
@@ -7894,7 +7894,7 @@
         <v>0.157713532678999</v>
       </c>
       <c r="N169" t="n">
-        <v>0.4473283034070282</v>
+        <v>0.3858994711917634</v>
       </c>
     </row>
     <row r="170">
@@ -7938,7 +7938,7 @@
         <v>0.6742385699656026</v>
       </c>
       <c r="N170" t="n">
-        <v>0.637638238817094</v>
+        <v>0.5417971284887391</v>
       </c>
     </row>
     <row r="171">
@@ -7982,7 +7982,7 @@
         <v>0.5852481844922746</v>
       </c>
       <c r="N171" t="n">
-        <v>0.4849422128700857</v>
+        <v>0.3687836824191397</v>
       </c>
     </row>
     <row r="172">
@@ -8026,7 +8026,7 @@
         <v>0.2695276053565618</v>
       </c>
       <c r="N172" t="n">
-        <v>-0.03759242905096578</v>
+        <v>0.1389961125822876</v>
       </c>
     </row>
     <row r="173">
@@ -8070,7 +8070,7 @@
         <v>0.4759268964377734</v>
       </c>
       <c r="N173" t="n">
-        <v>0.03598186863234236</v>
+        <v>0.2141823440786377</v>
       </c>
     </row>
     <row r="174">
@@ -8114,7 +8114,7 @@
         <v>0.728634669061778</v>
       </c>
       <c r="N174" t="n">
-        <v>0.6839138949626441</v>
+        <v>0.6959276757485893</v>
       </c>
     </row>
     <row r="175">
@@ -8158,7 +8158,7 @@
         <v>-0.8474844959459539</v>
       </c>
       <c r="N175" t="n">
-        <v>-0.9516247499381437</v>
+        <v>-0.9691884833702401</v>
       </c>
     </row>
     <row r="176">
@@ -8202,7 +8202,7 @@
         <v>0.5940174051775413</v>
       </c>
       <c r="N176" t="n">
-        <v>0.6315723941748724</v>
+        <v>0.6918078230721126</v>
       </c>
     </row>
     <row r="177">
@@ -8246,7 +8246,7 @@
         <v>0.7914651203060574</v>
       </c>
       <c r="N177" t="n">
-        <v>0.7542822754338258</v>
+        <v>0.8247471310121486</v>
       </c>
     </row>
     <row r="178">
@@ -8290,7 +8290,7 @@
         <v>0.5748052586855379</v>
       </c>
       <c r="N178" t="n">
-        <v>0.4849700116796447</v>
+        <v>0.7340996169055191</v>
       </c>
     </row>
     <row r="179">
@@ -8334,7 +8334,7 @@
         <v>-0.0332511268517687</v>
       </c>
       <c r="N179" t="n">
-        <v>0.080925555653254</v>
+        <v>0.3164913457952607</v>
       </c>
     </row>
     <row r="180">
@@ -8378,7 +8378,7 @@
         <v>-0.8077108381810748</v>
       </c>
       <c r="N180" t="n">
-        <v>-0.8437102954622027</v>
+        <v>-0.7536882432851889</v>
       </c>
     </row>
     <row r="181">
@@ -8422,7 +8422,7 @@
         <v>0.68164068078046</v>
       </c>
       <c r="N181" t="n">
-        <v>0.7676948049513512</v>
+        <v>0.7770470244085872</v>
       </c>
     </row>
     <row r="182">
@@ -8466,7 +8466,7 @@
         <v>0.6608774172208106</v>
       </c>
       <c r="N182" t="n">
-        <v>0.4628276630649954</v>
+        <v>0.606666289360147</v>
       </c>
     </row>
     <row r="183">
@@ -8510,7 +8510,7 @@
         <v>0.9269573826842872</v>
       </c>
       <c r="N183" t="n">
-        <v>0.939655496185164</v>
+        <v>0.9340571779843014</v>
       </c>
     </row>
     <row r="184">
@@ -8554,7 +8554,7 @@
         <v>-0.4134058702135761</v>
       </c>
       <c r="N184" t="n">
-        <v>-0.3028413763283749</v>
+        <v>-0.3005743533214336</v>
       </c>
     </row>
     <row r="185">
@@ -8598,7 +8598,7 @@
         <v>0.2393460149120048</v>
       </c>
       <c r="N185" t="n">
-        <v>0.5143809663200608</v>
+        <v>0.6133608290661291</v>
       </c>
     </row>
     <row r="186">
@@ -8642,7 +8642,7 @@
         <v>0.7457978514691315</v>
       </c>
       <c r="N186" t="n">
-        <v>0.4734946974421887</v>
+        <v>0.5671298389538912</v>
       </c>
     </row>
     <row r="187">
@@ -8686,7 +8686,7 @@
         <v>0.8390633627439612</v>
       </c>
       <c r="N187" t="n">
-        <v>0.8957849813402073</v>
+        <v>0.8750904845386713</v>
       </c>
     </row>
     <row r="188">
@@ -8730,7 +8730,7 @@
         <v>0.8182660245429301</v>
       </c>
       <c r="N188" t="n">
-        <v>0.8454419673357614</v>
+        <v>0.8534129902578838</v>
       </c>
     </row>
     <row r="189">
@@ -8774,7 +8774,7 @@
         <v>0.5988975713920465</v>
       </c>
       <c r="N189" t="n">
-        <v>0.7045819033039858</v>
+        <v>0.7445611741964537</v>
       </c>
     </row>
     <row r="190">
@@ -8818,7 +8818,7 @@
         <v>0.82710039380295</v>
       </c>
       <c r="N190" t="n">
-        <v>0.7084008934805854</v>
+        <v>0.7342055387355928</v>
       </c>
     </row>
     <row r="191">
@@ -8862,7 +8862,7 @@
         <v>-0.1867862879031699</v>
       </c>
       <c r="N191" t="n">
-        <v>-0.1766778321214958</v>
+        <v>-0.1014792482606526</v>
       </c>
     </row>
     <row r="192">
@@ -8906,7 +8906,7 @@
         <v>0.616504284574233</v>
       </c>
       <c r="N192" t="n">
-        <v>0.4550768020475844</v>
+        <v>0.4477930701235273</v>
       </c>
     </row>
     <row r="193">
@@ -8950,7 +8950,7 @@
         <v>0.8153260413925046</v>
       </c>
       <c r="N193" t="n">
-        <v>0.7997764161424918</v>
+        <v>0.830852655774197</v>
       </c>
     </row>
     <row r="194">
@@ -8994,7 +8994,7 @@
         <v>-0.7671083315192539</v>
       </c>
       <c r="N194" t="n">
-        <v>-0.7478331869181826</v>
+        <v>-0.7038439410703287</v>
       </c>
     </row>
     <row r="195">
@@ -9038,7 +9038,7 @@
         <v>0.8021960106857795</v>
       </c>
       <c r="N195" t="n">
-        <v>0.8482883201677002</v>
+        <v>0.8466229935809477</v>
       </c>
     </row>
     <row r="196">
@@ -9082,7 +9082,7 @@
         <v>0.8474486056674524</v>
       </c>
       <c r="N196" t="n">
-        <v>0.8638353835334884</v>
+        <v>0.8756730398829679</v>
       </c>
     </row>
     <row r="197">
@@ -9126,7 +9126,7 @@
         <v>0.0585330177224451</v>
       </c>
       <c r="N197" t="n">
-        <v>0.04891014108351034</v>
+        <v>0.07570887318006148</v>
       </c>
     </row>
     <row r="198">
@@ -9170,7 +9170,7 @@
         <v>-0.6079400781616185</v>
       </c>
       <c r="N198" t="n">
-        <v>-0.4842497468608122</v>
+        <v>-0.3655145275860947</v>
       </c>
     </row>
     <row r="199">
@@ -9214,7 +9214,7 @@
         <v>0.9103328514600668</v>
       </c>
       <c r="N199" t="n">
-        <v>0.9338742096846079</v>
+        <v>0.936238760431255</v>
       </c>
     </row>
     <row r="200">
@@ -9258,7 +9258,7 @@
         <v>0.7583111507514205</v>
       </c>
       <c r="N200" t="n">
-        <v>0.739061996732823</v>
+        <v>0.7486079887925494</v>
       </c>
     </row>
     <row r="201">
@@ -9302,7 +9302,7 @@
         <v>0.6865174666296797</v>
       </c>
       <c r="N201" t="n">
-        <v>0.6042984713287316</v>
+        <v>0.5447472121472136</v>
       </c>
     </row>
     <row r="202">
@@ -9346,7 +9346,7 @@
         <v>0.7764451628142132</v>
       </c>
       <c r="N202" t="n">
-        <v>0.769141853636694</v>
+        <v>0.7484416917351955</v>
       </c>
     </row>
     <row r="203">
@@ -9390,7 +9390,7 @@
         <v>-0.595943202604738</v>
       </c>
       <c r="N203" t="n">
-        <v>-0.5190999929150198</v>
+        <v>-0.4393824550708857</v>
       </c>
     </row>
     <row r="204">
@@ -9434,7 +9434,7 @@
         <v>0.7520566725291057</v>
       </c>
       <c r="N204" t="n">
-        <v>0.7707141290924567</v>
+        <v>0.7888468686020906</v>
       </c>
     </row>
     <row r="205">
@@ -9478,7 +9478,7 @@
         <v>0.7579168627253673</v>
       </c>
       <c r="N205" t="n">
-        <v>0.7820154266011687</v>
+        <v>0.80379765277825</v>
       </c>
     </row>
     <row r="206">
@@ -9522,7 +9522,7 @@
         <v>0.2240842749014155</v>
       </c>
       <c r="N206" t="n">
-        <v>-0.006484265171049788</v>
+        <v>0.0833349948368739</v>
       </c>
     </row>
     <row r="207">
@@ -9566,7 +9566,7 @@
         <v>0.7665116282305198</v>
       </c>
       <c r="N207" t="n">
-        <v>0.7273038894141867</v>
+        <v>0.7458841780586241</v>
       </c>
     </row>
     <row r="208">
@@ -9610,7 +9610,7 @@
         <v>0.7320024297431288</v>
       </c>
       <c r="N208" t="n">
-        <v>0.7349035944007156</v>
+        <v>0.7428248317023121</v>
       </c>
     </row>
     <row r="209">
@@ -9654,7 +9654,7 @@
         <v>0.730759972179748</v>
       </c>
       <c r="N209" t="n">
-        <v>0.7141476042507428</v>
+        <v>0.7313611919470593</v>
       </c>
     </row>
     <row r="210">
@@ -9698,7 +9698,7 @@
         <v>-0.7775787067071014</v>
       </c>
       <c r="N210" t="n">
-        <v>-0.7263435901487358</v>
+        <v>-0.6870957383155648</v>
       </c>
     </row>
     <row r="211">
@@ -9742,7 +9742,7 @@
         <v>0.8154644445397967</v>
       </c>
       <c r="N211" t="n">
-        <v>0.6112773471596396</v>
+        <v>0.4242192632937736</v>
       </c>
     </row>
     <row r="212">
@@ -9786,7 +9786,7 @@
         <v>-0.0221754607121119</v>
       </c>
       <c r="N212" t="n">
-        <v>0.2799405305916096</v>
+        <v>0.03506888300777106</v>
       </c>
     </row>
     <row r="213">
@@ -9830,7 +9830,7 @@
         <v>0.7732415166316593</v>
       </c>
       <c r="N213" t="n">
-        <v>0.7747724289148993</v>
+        <v>0.7540072017238539</v>
       </c>
     </row>
     <row r="214">
@@ -9874,7 +9874,7 @@
         <v>-0.1628521641581692</v>
       </c>
       <c r="N214" t="n">
-        <v>-0.2902595618868619</v>
+        <v>-0.2224073819899459</v>
       </c>
     </row>
     <row r="215">
@@ -9918,7 +9918,7 @@
         <v>-0.5503271278790477</v>
       </c>
       <c r="N215" t="n">
-        <v>-0.3326352217784836</v>
+        <v>-0.1720960065860631</v>
       </c>
     </row>
     <row r="216">
@@ -9962,7 +9962,7 @@
         <v>0.8313849364552758</v>
       </c>
       <c r="N216" t="n">
-        <v>0.8295656602793835</v>
+        <v>0.80749497552139</v>
       </c>
     </row>
     <row r="217">
@@ -10006,7 +10006,7 @@
         <v>0.7689807821289824</v>
       </c>
       <c r="N217" t="n">
-        <v>0.7564920692178579</v>
+        <v>0.7264754574251964</v>
       </c>
     </row>
     <row r="218">
@@ -10050,7 +10050,7 @@
         <v>0.7989802369473089</v>
       </c>
       <c r="N218" t="n">
-        <v>0.7841462696482271</v>
+        <v>0.7367704110837929</v>
       </c>
     </row>
     <row r="219">
@@ -10094,7 +10094,7 @@
         <v>-0.5558210820212334</v>
       </c>
       <c r="N219" t="n">
-        <v>-0.473182891331859</v>
+        <v>-0.29096806834264</v>
       </c>
     </row>
     <row r="220">
@@ -10138,7 +10138,7 @@
         <v>0.359278905755988</v>
       </c>
       <c r="N220" t="n">
-        <v>0.0130144257712001</v>
+        <v>0.07632867028008583</v>
       </c>
     </row>
     <row r="221">
@@ -10182,7 +10182,7 @@
         <v>0.75934295950968</v>
       </c>
       <c r="N221" t="n">
-        <v>0.7437444800133105</v>
+        <v>0.7482705350546481</v>
       </c>
     </row>
     <row r="222">
@@ -10226,7 +10226,7 @@
         <v>0.8570219538614862</v>
       </c>
       <c r="N222" t="n">
-        <v>0.8540165487198763</v>
+        <v>0.9038452771680123</v>
       </c>
     </row>
     <row r="223">
@@ -10270,7 +10270,7 @@
         <v>0.8257586739939377</v>
       </c>
       <c r="N223" t="n">
-        <v>0.8453139846060819</v>
+        <v>0.8274409817149182</v>
       </c>
     </row>
     <row r="224">
@@ -10314,7 +10314,7 @@
         <v>0.4825663444299294</v>
       </c>
       <c r="N224" t="n">
-        <v>0.3530306360066926</v>
+        <v>0.5606189084127275</v>
       </c>
     </row>
     <row r="225">
@@ -10358,7 +10358,7 @@
         <v>-0.7055048366253232</v>
       </c>
       <c r="N225" t="n">
-        <v>-0.7016636787711276</v>
+        <v>-0.7074045344279541</v>
       </c>
     </row>
     <row r="226">
@@ -10402,7 +10402,7 @@
         <v>0.4875730845458179</v>
       </c>
       <c r="N226" t="n">
-        <v>0.1877702153701715</v>
+        <v>-0.05131795611588519</v>
       </c>
     </row>
     <row r="227">
@@ -10446,7 +10446,7 @@
         <v>0.8889501993116453</v>
       </c>
       <c r="N227" t="n">
-        <v>0.9045453115359575</v>
+        <v>0.9090317404018262</v>
       </c>
     </row>
     <row r="228">
@@ -10490,7 +10490,7 @@
         <v>0.8645684620336349</v>
       </c>
       <c r="N228" t="n">
-        <v>0.8592645542078898</v>
+        <v>0.8566193421995973</v>
       </c>
     </row>
     <row r="229">
@@ -10534,7 +10534,7 @@
         <v>0.8043834523637883</v>
       </c>
       <c r="N229" t="n">
-        <v>0.8115640992404366</v>
+        <v>0.7803794279349179</v>
       </c>
     </row>
     <row r="230">
@@ -10578,7 +10578,7 @@
         <v>0.8657677372848187</v>
       </c>
       <c r="N230" t="n">
-        <v>0.8860733208890237</v>
+        <v>0.8661002035059793</v>
       </c>
     </row>
     <row r="231">
@@ -10622,7 +10622,7 @@
         <v>0.552911133144269</v>
       </c>
       <c r="N231" t="n">
-        <v>0.6455952291083842</v>
+        <v>0.7400058807357832</v>
       </c>
     </row>
     <row r="232">
@@ -10666,7 +10666,7 @@
         <v>0.8104896677349587</v>
       </c>
       <c r="N232" t="n">
-        <v>0.8323072461675941</v>
+        <v>0.8052361245475148</v>
       </c>
     </row>
     <row r="233">
@@ -10710,7 +10710,7 @@
         <v>0.7739471668964308</v>
       </c>
       <c r="N233" t="n">
-        <v>0.6478134881281663</v>
+        <v>0.6216818923801425</v>
       </c>
     </row>
     <row r="234">
@@ -10754,7 +10754,7 @@
         <v>0.8248296341644575</v>
       </c>
       <c r="N234" t="n">
-        <v>0.832048804137149</v>
+        <v>0.8169278579100039</v>
       </c>
     </row>
     <row r="235">
@@ -10798,7 +10798,7 @@
         <v>-0.7793900622438272</v>
       </c>
       <c r="N235" t="n">
-        <v>-0.8990845228611609</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="236">
@@ -10842,7 +10842,7 @@
         <v>-0.3641366460900203</v>
       </c>
       <c r="N236" t="n">
-        <v>-0.3263838037441186</v>
+        <v>-0.1634194336052662</v>
       </c>
     </row>
     <row r="237">
@@ -10886,7 +10886,7 @@
         <v>0.6067083447251046</v>
       </c>
       <c r="N237" t="n">
-        <v>0.6885949909551691</v>
+        <v>0.757567659943947</v>
       </c>
     </row>
     <row r="238">
@@ -10930,7 +10930,7 @@
         <v>0.8212654376490229</v>
       </c>
       <c r="N238" t="n">
-        <v>0.8468133715401751</v>
+        <v>0.8211508439472287</v>
       </c>
     </row>
     <row r="239">
@@ -10974,7 +10974,7 @@
         <v>0.7587488106997804</v>
       </c>
       <c r="N239" t="n">
-        <v>0.6461868829534382</v>
+        <v>0.6688936947444915</v>
       </c>
     </row>
     <row r="240">
@@ -11018,7 +11018,7 @@
         <v>-0.4707242007927845</v>
       </c>
       <c r="N240" t="n">
-        <v>-0.5200730087688825</v>
+        <v>-0.2805208381850709</v>
       </c>
     </row>
     <row r="241">
@@ -11062,7 +11062,7 @@
         <v>-0.1812453134125466</v>
       </c>
       <c r="N241" t="n">
-        <v>-0.254267147587386</v>
+        <v>-0.1663209236216885</v>
       </c>
     </row>
     <row r="242">
@@ -11106,7 +11106,7 @@
         <v>-0.2376381757008022</v>
       </c>
       <c r="N242" t="n">
-        <v>-0.1393488808204423</v>
+        <v>-0.07667922303084562</v>
       </c>
     </row>
     <row r="243">
@@ -11150,7 +11150,7 @@
         <v>-0.7998247873514476</v>
       </c>
       <c r="N243" t="n">
-        <v>-0.7826475961561249</v>
+        <v>-0.7597401775565683</v>
       </c>
     </row>
     <row r="244">
@@ -11194,7 +11194,7 @@
         <v>-0.7195127148028737</v>
       </c>
       <c r="N244" t="n">
-        <v>-0.7269703054065892</v>
+        <v>-0.7245202810970407</v>
       </c>
     </row>
     <row r="245">
@@ -11238,7 +11238,7 @@
         <v>0.5174946650034078</v>
       </c>
       <c r="N245" t="n">
-        <v>0.374303079071753</v>
+        <v>0.4282300089889726</v>
       </c>
     </row>
     <row r="246">
@@ -11282,7 +11282,7 @@
         <v>0.5926949962463273</v>
       </c>
       <c r="N246" t="n">
-        <v>0.5875577982202482</v>
+        <v>0.6195752450824312</v>
       </c>
     </row>
     <row r="247">
@@ -11326,7 +11326,7 @@
         <v>-0.2592504403852613</v>
       </c>
       <c r="N247" t="n">
-        <v>0.02288562127451872</v>
+        <v>-0.07590877354017889</v>
       </c>
     </row>
     <row r="248">
@@ -11370,7 +11370,7 @@
         <v>-0.7013244455498588</v>
       </c>
       <c r="N248" t="n">
-        <v>-0.5667152267906013</v>
+        <v>-0.5951601303896258</v>
       </c>
     </row>
     <row r="249">
@@ -11414,7 +11414,7 @@
         <v>0.8323845596200692</v>
       </c>
       <c r="N249" t="n">
-        <v>0.8529218783577518</v>
+        <v>0.8645871146946439</v>
       </c>
     </row>
     <row r="250">
@@ -11458,7 +11458,7 @@
         <v>-0.6826331580445066</v>
       </c>
       <c r="N250" t="n">
-        <v>-0.6741420500932226</v>
+        <v>-0.6545056347049875</v>
       </c>
     </row>
     <row r="251">
@@ -11502,7 +11502,7 @@
         <v>0.9164307800053916</v>
       </c>
       <c r="N251" t="n">
-        <v>1</v>
+        <v>0.9777516194794389</v>
       </c>
     </row>
     <row r="252">
@@ -11546,7 +11546,7 @@
         <v>0.7768412654500212</v>
       </c>
       <c r="N252" t="n">
-        <v>0.7722266038544071</v>
+        <v>0.7659443866104503</v>
       </c>
     </row>
     <row r="253">
@@ -11590,7 +11590,7 @@
         <v>0.7801902617599272</v>
       </c>
       <c r="N253" t="n">
-        <v>0.847689272231399</v>
+        <v>0.8431553817226026</v>
       </c>
     </row>
     <row r="254">
@@ -11634,7 +11634,7 @@
         <v>0.722118320733084</v>
       </c>
       <c r="N254" t="n">
-        <v>0.6418781560964404</v>
+        <v>0.6540447808680624</v>
       </c>
     </row>
     <row r="255">
@@ -11678,7 +11678,7 @@
         <v>-0.6596489699491949</v>
       </c>
       <c r="N255" t="n">
-        <v>-0.5242788339351493</v>
+        <v>-0.6217899476252583</v>
       </c>
     </row>
     <row r="256">
@@ -11722,7 +11722,7 @@
         <v>0.7225372419611462</v>
       </c>
       <c r="N256" t="n">
-        <v>0.6010538386270264</v>
+        <v>0.3963718844949579</v>
       </c>
     </row>
     <row r="257">
@@ -11766,7 +11766,7 @@
         <v>0.7461628806620854</v>
       </c>
       <c r="N257" t="n">
-        <v>0.7047068285837366</v>
+        <v>0.7576226806531126</v>
       </c>
     </row>
     <row r="258">
@@ -11810,7 +11810,7 @@
         <v>-0.7329665350452134</v>
       </c>
       <c r="N258" t="n">
-        <v>-0.6707798107019364</v>
+        <v>-0.7301455519394576</v>
       </c>
     </row>
     <row r="259">
@@ -11854,7 +11854,7 @@
         <v>0.5769730361773093</v>
       </c>
       <c r="N259" t="n">
-        <v>0.6155397897085633</v>
+        <v>0.6766911058391506</v>
       </c>
     </row>
     <row r="260">
@@ -11898,7 +11898,7 @@
         <v>0.8930400952240134</v>
       </c>
       <c r="N260" t="n">
-        <v>0.89683474823775</v>
+        <v>0.9013414141825498</v>
       </c>
     </row>
     <row r="261">
@@ -11942,7 +11942,7 @@
         <v>0.9067997849402027</v>
       </c>
       <c r="N261" t="n">
-        <v>0.9605885461481527</v>
+        <v>0.9431491625691755</v>
       </c>
     </row>
     <row r="262">
@@ -11986,7 +11986,7 @@
         <v>0.2466385010284907</v>
       </c>
       <c r="N262" t="n">
-        <v>0.5614155405302764</v>
+        <v>0.3029988518813714</v>
       </c>
     </row>
     <row r="263">
@@ -12030,7 +12030,7 @@
         <v>0.7025971916154194</v>
       </c>
       <c r="N263" t="n">
-        <v>0.6188363278489896</v>
+        <v>0.6428942473847208</v>
       </c>
     </row>
     <row r="264">
@@ -12074,7 +12074,7 @@
         <v>0.7656968964466506</v>
       </c>
       <c r="N264" t="n">
-        <v>0.7969702297719152</v>
+        <v>0.7846654219423279</v>
       </c>
     </row>
     <row r="265">
@@ -12118,7 +12118,7 @@
         <v>0.6357006356070402</v>
       </c>
       <c r="N265" t="n">
-        <v>-0.2381005491807709</v>
+        <v>-0.05743722578343591</v>
       </c>
     </row>
     <row r="266">
@@ -12162,7 +12162,7 @@
         <v>0.9123284708103654</v>
       </c>
       <c r="N266" t="n">
-        <v>0.9090123855774884</v>
+        <v>0.9016156611334027</v>
       </c>
     </row>
     <row r="267">
@@ -12206,7 +12206,7 @@
         <v>0.8490615614820165</v>
       </c>
       <c r="N267" t="n">
-        <v>0.8604687688412899</v>
+        <v>0.8413734960741963</v>
       </c>
     </row>
     <row r="268">
@@ -12250,7 +12250,7 @@
         <v>0.8675793731570087</v>
       </c>
       <c r="N268" t="n">
-        <v>0.9140347827659683</v>
+        <v>0.9240942146038447</v>
       </c>
     </row>
     <row r="269">
@@ -12294,7 +12294,7 @@
         <v>0.8571725672626157</v>
       </c>
       <c r="N269" t="n">
-        <v>0.9063713625404392</v>
+        <v>0.877176212803655</v>
       </c>
     </row>
     <row r="270">
@@ -12338,7 +12338,7 @@
         <v>-0.3078632895784172</v>
       </c>
       <c r="N270" t="n">
-        <v>-0.2828893149488836</v>
+        <v>-0.2074894963982643</v>
       </c>
     </row>
     <row r="271">
@@ -12382,7 +12382,7 @@
         <v>0.5167035481707074</v>
       </c>
       <c r="N271" t="n">
-        <v>0.4777184401868844</v>
+        <v>0.3691517263917865</v>
       </c>
     </row>
     <row r="272">
@@ -12426,7 +12426,7 @@
         <v>-0.0252525471168636</v>
       </c>
       <c r="N272" t="n">
-        <v>0.1404795565413993</v>
+        <v>0.08399177598691138</v>
       </c>
     </row>
     <row r="273">
@@ -12470,7 +12470,7 @@
         <v>0.7982155898796746</v>
       </c>
       <c r="N273" t="n">
-        <v>0.7876806880189773</v>
+        <v>0.7982601512476855</v>
       </c>
     </row>
     <row r="274">
@@ -12514,7 +12514,7 @@
         <v>0.8412691889104932</v>
       </c>
       <c r="N274" t="n">
-        <v>0.8501071196757168</v>
+        <v>0.8216613581577175</v>
       </c>
     </row>
     <row r="275">
@@ -12558,7 +12558,7 @@
         <v>0.1767508522070731</v>
       </c>
       <c r="N275" t="n">
-        <v>0.3350706203051087</v>
+        <v>0.1057665185130325</v>
       </c>
     </row>
     <row r="276">
@@ -12602,7 +12602,7 @@
         <v>0.724745312172117</v>
       </c>
       <c r="N276" t="n">
-        <v>0.6490546852799346</v>
+        <v>0.6786688411469297</v>
       </c>
     </row>
     <row r="277">
@@ -12646,7 +12646,7 @@
         <v>0.9433082394212972</v>
       </c>
       <c r="N277" t="n">
-        <v>1</v>
+        <v>0.9917264745548762</v>
       </c>
     </row>
     <row r="278">
@@ -12690,7 +12690,7 @@
         <v>-0.2552088315941675</v>
       </c>
       <c r="N278" t="n">
-        <v>0.08268827115828965</v>
+        <v>-0.1407306961669953</v>
       </c>
     </row>
     <row r="279">
@@ -12734,7 +12734,7 @@
         <v>0.2661160453093643</v>
       </c>
       <c r="N279" t="n">
-        <v>0.5982178510248656</v>
+        <v>0.3329546162692637</v>
       </c>
     </row>
     <row r="280">
@@ -12778,7 +12778,7 @@
         <v>0.8160584047082554</v>
       </c>
       <c r="N280" t="n">
-        <v>0.7994591005657909</v>
+        <v>0.7697110759003355</v>
       </c>
     </row>
     <row r="281">
@@ -12822,7 +12822,7 @@
         <v>0.9246780502892864</v>
       </c>
       <c r="N281" t="n">
-        <v>0.7640363792115743</v>
+        <v>0.7604817748035375</v>
       </c>
     </row>
     <row r="282">
@@ -12866,7 +12866,7 @@
         <v>0.7897378170636717</v>
       </c>
       <c r="N282" t="n">
-        <v>0.8468812991175761</v>
+        <v>0.8298213640927815</v>
       </c>
     </row>
     <row r="283">
@@ -12910,7 +12910,7 @@
         <v>-0.0841485201365562</v>
       </c>
       <c r="N283" t="n">
-        <v>-0.08607308135170881</v>
+        <v>0.2144863847353026</v>
       </c>
     </row>
     <row r="284">
@@ -12954,7 +12954,7 @@
         <v>0.8033797220679606</v>
       </c>
       <c r="N284" t="n">
-        <v>0.7769112656173505</v>
+        <v>0.7845871274675769</v>
       </c>
     </row>
     <row r="285">
@@ -12998,7 +12998,7 @@
         <v>0.8074963036045859</v>
       </c>
       <c r="N285" t="n">
-        <v>0.8215728465067289</v>
+        <v>0.8416948424243218</v>
       </c>
     </row>
     <row r="286">
@@ -13042,7 +13042,7 @@
         <v>0.6665928179830543</v>
       </c>
       <c r="N286" t="n">
-        <v>0.5388874733278466</v>
+        <v>0.2457452524832795</v>
       </c>
     </row>
     <row r="287">
@@ -13086,7 +13086,7 @@
         <v>0.6337178345509416</v>
       </c>
       <c r="N287" t="n">
-        <v>0.7083144938553514</v>
+        <v>0.7523360548820217</v>
       </c>
     </row>
     <row r="288">
@@ -13130,7 +13130,7 @@
         <v>0.8132345320475391</v>
       </c>
       <c r="N288" t="n">
-        <v>0.8273400655851553</v>
+        <v>0.8327233861036061</v>
       </c>
     </row>
     <row r="289">
@@ -13174,7 +13174,7 @@
         <v>0.840902066112066</v>
       </c>
       <c r="N289" t="n">
-        <v>0.6935310446572793</v>
+        <v>0.6665733198434447</v>
       </c>
     </row>
     <row r="290">
@@ -13218,7 +13218,7 @@
         <v>0.7058091043262783</v>
       </c>
       <c r="N290" t="n">
-        <v>0.367740205701761</v>
+        <v>0.4047474240448911</v>
       </c>
     </row>
     <row r="291">
@@ -13262,7 +13262,7 @@
         <v>-0.1044128956207703</v>
       </c>
       <c r="N291" t="n">
-        <v>-0.01490054567598829</v>
+        <v>0.1151053847881202</v>
       </c>
     </row>
     <row r="292">
@@ -13306,7 +13306,7 @@
         <v>0.8435825471644358</v>
       </c>
       <c r="N292" t="n">
-        <v>0.8251501317434026</v>
+        <v>0.7817870959717612</v>
       </c>
     </row>
     <row r="293">
@@ -13350,7 +13350,7 @@
         <v>-0.7407396864315133</v>
       </c>
       <c r="N293" t="n">
-        <v>-0.7735893963812686</v>
+        <v>-0.7883708861216</v>
       </c>
     </row>
     <row r="294">
@@ -13394,7 +13394,7 @@
         <v>-0.1592253620417615</v>
       </c>
       <c r="N294" t="n">
-        <v>-0.1851293499639513</v>
+        <v>-0.13320714842559</v>
       </c>
     </row>
     <row r="295">
@@ -13438,7 +13438,7 @@
         <v>0.8155485262274341</v>
       </c>
       <c r="N295" t="n">
-        <v>0.8193381383154554</v>
+        <v>0.8203730663345965</v>
       </c>
     </row>
     <row r="296">
@@ -13482,7 +13482,7 @@
         <v>-0.8602061959300022</v>
       </c>
       <c r="N296" t="n">
-        <v>-0.9409854290290928</v>
+        <v>-0.9180390502923063</v>
       </c>
     </row>
     <row r="297">
@@ -13526,7 +13526,7 @@
         <v>0.8759237408454921</v>
       </c>
       <c r="N297" t="n">
-        <v>0.871417265996432</v>
+        <v>0.8892270788555854</v>
       </c>
     </row>
     <row r="298">
@@ -13570,7 +13570,7 @@
         <v>-0.7677695239702951</v>
       </c>
       <c r="N298" t="n">
-        <v>-0.8131458024351931</v>
+        <v>-0.793357324878614</v>
       </c>
     </row>
     <row r="299">
@@ -13614,7 +13614,7 @@
         <v>-0.3493320514589051</v>
       </c>
       <c r="N299" t="n">
-        <v>-0.3168825017825962</v>
+        <v>-0.2931745550448445</v>
       </c>
     </row>
     <row r="300">
@@ -13658,7 +13658,7 @@
         <v>0.9410932091563624</v>
       </c>
       <c r="N300" t="n">
-        <v>0.9874323723544389</v>
+        <v>0.9593292270563722</v>
       </c>
     </row>
     <row r="301">
@@ -13702,7 +13702,7 @@
         <v>-0.7868710726850842</v>
       </c>
       <c r="N301" t="n">
-        <v>-0.7951451718254419</v>
+        <v>-0.7609228068855901</v>
       </c>
     </row>
     <row r="302">
@@ -13746,7 +13746,7 @@
         <v>-0.4417337361166677</v>
       </c>
       <c r="N302" t="n">
-        <v>-0.2542314041375017</v>
+        <v>-0.1851351364745429</v>
       </c>
     </row>
     <row r="303">
@@ -13790,7 +13790,7 @@
         <v>-0.5266137891910706</v>
       </c>
       <c r="N303" t="n">
-        <v>-0.332352699074749</v>
+        <v>-0.221894389471965</v>
       </c>
     </row>
     <row r="304">
@@ -13834,7 +13834,7 @@
         <v>-0.6113979268202668</v>
       </c>
       <c r="N304" t="n">
-        <v>-0.524028203018545</v>
+        <v>-0.4825132957913264</v>
       </c>
     </row>
     <row r="305">
@@ -13878,7 +13878,7 @@
         <v>0.773140224167277</v>
       </c>
       <c r="N305" t="n">
-        <v>0.7861864821395494</v>
+        <v>0.7941069936195468</v>
       </c>
     </row>
     <row r="306">
@@ -13922,7 +13922,7 @@
         <v>0.6270403054581494</v>
       </c>
       <c r="N306" t="n">
-        <v>0.5802525335823834</v>
+        <v>0.7014254762517029</v>
       </c>
     </row>
     <row r="307">
@@ -13966,7 +13966,7 @@
         <v>-0.4863216298340837</v>
       </c>
       <c r="N307" t="n">
-        <v>-0.4432469197090613</v>
+        <v>-0.4265578093283714</v>
       </c>
     </row>
     <row r="308">
@@ -14010,7 +14010,7 @@
         <v>0.6927980063457103</v>
       </c>
       <c r="N308" t="n">
-        <v>0.6294041191843706</v>
+        <v>0.587380301807794</v>
       </c>
     </row>
     <row r="309">
@@ -14054,7 +14054,7 @@
         <v>0.4661309450996959</v>
       </c>
       <c r="N309" t="n">
-        <v>0.6151699564092126</v>
+        <v>0.6725863457271968</v>
       </c>
     </row>
   </sheetData>

</xml_diff>